<commit_message>
Communication betwen Nextion displayn and Arduino is working! Also added a flowchart to the Arduino main Program.
</commit_message>
<xml_diff>
--- a/Documents/CocktailRecipes.xlsx
+++ b/Documents/CocktailRecipes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weiss\Desktop\Ntj\Basteln\CM\DesignIdeas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weiss\Desktop\Ntj\Basteln\CM\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD709F4-F211-4E84-AD6D-FF8FDF8AEAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F47EDA-16D7-4BC1-BF7B-3765AF614F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="368" windowWidth="12300" windowHeight="15112" xr2:uid="{2E45057B-C607-4832-86B0-13D1CA8A00A0}"/>
+    <workbookView xWindow="18690" yWindow="1477" windowWidth="18225" windowHeight="11386" xr2:uid="{2E45057B-C607-4832-86B0-13D1CA8A00A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1764E81F-47FA-4F5B-8876-76DF704625A9}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>